<commit_message>
Added missing Facebook data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\se-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC4D74F-0D2D-483B-9442-A583713D6824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DCBB00-3D2E-4388-9D6F-D715030E4BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5820" yWindow="2805" windowWidth="12150" windowHeight="11880" activeTab="1" xr2:uid="{51A2F36B-B56E-4DB6-9E73-4DAB676C1519}"/>
+    <workbookView xWindow="0" yWindow="2805" windowWidth="12150" windowHeight="11880" activeTab="1" xr2:uid="{51A2F36B-B56E-4DB6-9E73-4DAB676C1519}"/>
   </bookViews>
   <sheets>
     <sheet name="resources" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
   <si>
     <t>SE Latest Release Playlist</t>
   </si>
@@ -254,6 +254,30 @@
   </si>
   <si>
     <t>https://twitter.com/StEpistemology</t>
+  </si>
+  <si>
+    <t>Facebook "Chat With a Street Epistemologist" Group</t>
+  </si>
+  <si>
+    <t>This group is for facilitating SE discussions over particular beliefs.</t>
+  </si>
+  <si>
+    <t>Facebook Critique SE Group</t>
+  </si>
+  <si>
+    <t>Public SE Facebook Page</t>
+  </si>
+  <si>
+    <t>This group is for raising and discussing any critiques of SE so that we can further learn about and improve the method.</t>
+  </si>
+  <si>
+    <t>A public page for believers and non-believers to discuss topics related to Street Epistemology.</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/ChatWithAStreetEpistemologist/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/StreetEpistemology</t>
   </si>
 </sst>
 </file>
@@ -934,10 +958,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C07A414-2AB9-4D5C-97D9-9E67270455B7}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E6"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +1008,7 @@
         <v>58</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E6" si="0">"{
+        <f t="shared" ref="E2:E9" si="0">"{
     logo: """ &amp; A2 &amp; """,
     title: """ &amp; B2 &amp; """,
     description: """ &amp; SUBSTITUTE(C2,"""","\""") &amp; """,
@@ -1090,6 +1114,75 @@
 },</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>{
+    logo: "logo_facebook",
+    title: "Facebook "Chat With a Street Epistemologist" Group",
+    description: "This group is for facilitating SE discussions over particular beliefs.",
+    url: "https://www.facebook.com/groups/ChatWithAStreetEpistemologist/"
+},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>{
+    logo: "logo_facebook",
+    title: "Facebook Critique SE Group",
+    description: "This group is for raising and discussing any critiques of SE so that we can further learn about and improve the method.",
+    url: "https://www.facebook.com/groups/ChatWithAStreetEpistemologist/"
+},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>{
+    logo: "logo_facebook",
+    title: "Public SE Facebook Page",
+    description: "A public page for believers and non-believers to discuss topics related to Street Epistemology.",
+    url: "https://www.facebook.com/StreetEpistemology"
+},</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>